<commit_message>
Customised xlsx-chart library. Fork present in TimeInc repo.
</commit_message>
<xml_diff>
--- a/template/column.xlsx
+++ b/template/column.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="18135" windowHeight="7170"/>
+    <workbookView xWindow="120" yWindow="140" windowWidth="28680" windowHeight="17400"/>
   </bookViews>
   <sheets>
     <sheet name="Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Table" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,8 +40,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,7 +75,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -79,13 +84,25 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="ru-RU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -100,6 +117,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Table!$A$2:$A$4</c:f>
@@ -124,13 +142,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -150,6 +168,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Table!$A$2:$A$4</c:f>
@@ -174,44 +193,60 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="49222784"/>
-        <c:axId val="49224320"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2055286200"/>
+        <c:axId val="2130973576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49222784"/>
+        <c:axId val="2055286200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49224320"/>
+        <c:crossAx val="2130973576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49224320"/>
+        <c:axId val="2130973576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49222784"/>
+        <c:crossAx val="2055286200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -219,8 +254,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -235,14 +273,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>101601</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:colOff>374651</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -260,6 +298,44 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1422400" y="76200"/>
+          <a:ext cx="5003800" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -549,27 +625,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
@@ -614,5 +695,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>